<commit_message>
modify the implementation of the xls export
</commit_message>
<xml_diff>
--- a/public/template.xlsx
+++ b/public/template.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t xml:space="preserve">Formular ore suplimentare</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t xml:space="preserve">Month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March</t>
   </si>
   <si>
     <t xml:space="preserve">Date of call</t>
@@ -538,18 +541,18 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8:E21"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.8866396761134"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.2834008097166"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="37.8137651821862"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="38.3481781376518"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -593,25 +596,24 @@
       <c r="B4" s="6"/>
       <c r="C4" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43175</v>
+        <v>43187</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="6"/>
-      <c r="C5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="4" t="str">
-        <f aca="false">TEXT(C4,"mmmm")</f>
-        <v>March</v>
-      </c>
+      <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -625,25 +627,25 @@
     </row>
     <row r="7" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -654,7 +656,10 @@
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
-      <c r="E8" s="13"/>
+      <c r="E8" s="13" t="str">
+        <f aca="false">IF(ISBLANK(C8),"",D8-C8)</f>
+        <v/>
+      </c>
       <c r="F8" s="14"/>
       <c r="G8" s="9"/>
     </row>
@@ -666,7 +671,10 @@
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
-      <c r="E9" s="13"/>
+      <c r="E9" s="13" t="str">
+        <f aca="false">IF(ISBLANK(C9),"",D9-C9)</f>
+        <v/>
+      </c>
       <c r="F9" s="14"/>
       <c r="G9" s="9"/>
     </row>
@@ -678,7 +686,10 @@
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
-      <c r="E10" s="13"/>
+      <c r="E10" s="13" t="str">
+        <f aca="false">IF(ISBLANK(C10),"",D10-C10)</f>
+        <v/>
+      </c>
       <c r="F10" s="14"/>
       <c r="G10" s="15"/>
     </row>
@@ -690,7 +701,10 @@
       </c>
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
-      <c r="E11" s="13"/>
+      <c r="E11" s="13" t="str">
+        <f aca="false">IF(ISBLANK(C11),"",D11-C11)</f>
+        <v/>
+      </c>
       <c r="F11" s="14"/>
       <c r="G11" s="16"/>
     </row>
@@ -702,7 +716,10 @@
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
-      <c r="E12" s="13"/>
+      <c r="E12" s="13" t="str">
+        <f aca="false">IF(ISBLANK(C12),"",D12-C12)</f>
+        <v/>
+      </c>
       <c r="F12" s="14"/>
       <c r="G12" s="16"/>
     </row>
@@ -714,7 +731,10 @@
       </c>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
-      <c r="E13" s="13"/>
+      <c r="E13" s="13" t="str">
+        <f aca="false">IF(ISBLANK(C13),"",D13-C13)</f>
+        <v/>
+      </c>
       <c r="F13" s="14"/>
       <c r="G13" s="9"/>
     </row>
@@ -726,7 +746,10 @@
       </c>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
-      <c r="E14" s="13"/>
+      <c r="E14" s="13" t="str">
+        <f aca="false">IF(ISBLANK(C14),"",D14-C14)</f>
+        <v/>
+      </c>
       <c r="F14" s="14"/>
       <c r="G14" s="9"/>
     </row>
@@ -738,7 +761,10 @@
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
-      <c r="E15" s="13"/>
+      <c r="E15" s="13" t="str">
+        <f aca="false">IF(ISBLANK(C15),"",D15-C15)</f>
+        <v/>
+      </c>
       <c r="F15" s="14"/>
       <c r="G15" s="15"/>
     </row>
@@ -750,7 +776,10 @@
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
-      <c r="E16" s="13"/>
+      <c r="E16" s="13" t="str">
+        <f aca="false">IF(ISBLANK(C16),"",D16-C16)</f>
+        <v/>
+      </c>
       <c r="F16" s="14"/>
       <c r="G16" s="16"/>
     </row>
@@ -762,7 +791,10 @@
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
-      <c r="E17" s="13"/>
+      <c r="E17" s="13" t="str">
+        <f aca="false">IF(ISBLANK(C17),"",D17-C17)</f>
+        <v/>
+      </c>
       <c r="F17" s="14"/>
       <c r="G17" s="16"/>
     </row>
@@ -774,7 +806,10 @@
       </c>
       <c r="C18" s="12"/>
       <c r="D18" s="12"/>
-      <c r="E18" s="13"/>
+      <c r="E18" s="13" t="str">
+        <f aca="false">IF(ISBLANK(C18),"",D18-C18)</f>
+        <v/>
+      </c>
       <c r="F18" s="14"/>
       <c r="G18" s="16"/>
     </row>
@@ -786,7 +821,10 @@
       </c>
       <c r="C19" s="12"/>
       <c r="D19" s="12"/>
-      <c r="E19" s="13"/>
+      <c r="E19" s="13" t="str">
+        <f aca="false">IF(ISBLANK(C19),"",D19-C19)</f>
+        <v/>
+      </c>
       <c r="F19" s="14"/>
       <c r="G19" s="16"/>
     </row>
@@ -798,7 +836,10 @@
       </c>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
-      <c r="E20" s="13"/>
+      <c r="E20" s="13" t="str">
+        <f aca="false">IF(ISBLANK(C20),"",D20-C20)</f>
+        <v/>
+      </c>
       <c r="F20" s="14"/>
       <c r="G20" s="16"/>
     </row>
@@ -810,7 +851,10 @@
       </c>
       <c r="C21" s="12"/>
       <c r="D21" s="12"/>
-      <c r="E21" s="13"/>
+      <c r="E21" s="13" t="str">
+        <f aca="false">IF(ISBLANK(C21),"",D21-C21)</f>
+        <v/>
+      </c>
       <c r="F21" s="14"/>
       <c r="G21" s="16"/>
     </row>
@@ -825,7 +869,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B23" s="19"/>
       <c r="C23" s="20" t="e">
@@ -842,7 +886,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B24" s="19"/>
       <c r="C24" s="20" t="e">
@@ -859,7 +903,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="23" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B25" s="23"/>
       <c r="C25" s="24"/>
@@ -882,17 +926,17 @@
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="27" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B27" s="27"/>
       <c r="C27" s="27"/>
       <c r="D27" s="28" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E27" s="28"/>
       <c r="F27" s="28"/>
       <c r="G27" s="29" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -903,12 +947,12 @@
       <c r="B28" s="30"/>
       <c r="C28" s="30"/>
       <c r="D28" s="31" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E28" s="31"/>
       <c r="F28" s="31"/>
       <c r="G28" s="32" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -921,11 +965,12 @@
       <c r="G29" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:G5"/>
     <mergeCell ref="D23:F23"/>
     <mergeCell ref="D24:F24"/>
     <mergeCell ref="A27:C27"/>
@@ -959,7 +1004,7 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="E8:E21 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1178,12 +1223,12 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="E8:E21 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>

</xml_diff>